<commit_message>
Starting direction classifaction module & improving unit number ocr
</commit_message>
<xml_diff>
--- a/unit_testing/unit_number_direction.xlsx
+++ b/unit_testing/unit_number_direction.xlsx
@@ -485,52 +485,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Unit Number</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_1_4</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>01;12</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_38_1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>;;</t>
-        </is>
-      </c>
+      <c r="A1" s="3" t="n"/>
+      <c r="B1" s="3" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_42_6</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>06;04;06;06</t>
-        </is>
-      </c>
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="n"/>
       <c r="C4" s="1" t="n"/>
     </row>
   </sheetData>
@@ -544,7 +504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
@@ -553,135 +513,16 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>Unit Number</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Direction</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>Image Name</t>
-        </is>
-      </c>
+      <c r="A1" s="3" t="n"/>
+      <c r="B1" s="3" t="n"/>
+      <c r="C1" s="3" t="n"/>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>south</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_1_4.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>12</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>south</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_1_4.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>8</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>north-east</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_38_1.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>north</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_42_6.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>west</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_42_6.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>north</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_42_6.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>north</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_42_6.jpg</t>
-        </is>
-      </c>
-    </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
removed gpt from direct classification
</commit_message>
<xml_diff>
--- a/unit_testing/unit_number_direction.xlsx
+++ b/unit_testing/unit_number_direction.xlsx
@@ -556,7 +556,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
@@ -565,160 +565,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>Unit Number</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Direction</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>Image Name</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>10</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>east</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_1_1.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>west</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_1_1.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>west</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_1_1.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>south</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_1_7.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>north</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_42_1.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>north</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_42_1.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>3</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>north</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_42_1.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>north-west</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_42_4.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>north-west</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_42_4.jpg</t>
-        </is>
-      </c>
+      <c r="A1" s="3" t="n"/>
+      <c r="B1" s="3" t="n"/>
+      <c r="C1" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
solved delete bug for CNN model main.py
</commit_message>
<xml_diff>
--- a/unit_testing/unit_number_direction.xlsx
+++ b/unit_testing/unit_number_direction.xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="A1:C7"/>
@@ -521,29 +521,9 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_42_1</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>03;03;03</t>
-        </is>
-      </c>
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="n"/>
       <c r="C4" s="1" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_42_4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1;1;</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
changed CRAFT folder creation;train with not aug
</commit_message>
<xml_diff>
--- a/unit_testing/unit_number_direction.xlsx
+++ b/unit_testing/unit_number_direction.xlsx
@@ -508,21 +508,9 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_1_7</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
-    </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr"/>
-      <c r="B4" s="1" t="inlineStr"/>
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="n"/>
       <c r="C4" s="1" t="n"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sorting for unit num ocr to resolve bug with dif coords
</commit_message>
<xml_diff>
--- a/unit_testing/unit_number_direction.xlsx
+++ b/unit_testing/unit_number_direction.xlsx
@@ -485,28 +485,8 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Unit Number</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>pdf_floor_plan_1_1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>10;04;03</t>
-        </is>
-      </c>
+      <c r="A1" s="3" t="n"/>
+      <c r="B1" s="3" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>

</xml_diff>